<commit_message>
saving comments in local storage
</commit_message>
<xml_diff>
--- a/alarm_rename.xlsx
+++ b/alarm_rename.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7095cc4eb6d386e0/Desktop/Alarms Filter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{A07BB8BF-9384-4330-9CAC-3D417C95C197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C928ADCE-53D8-41C5-9569-FAD4C36B5ECE}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{A07BB8BF-9384-4330-9CAC-3D417C95C197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07EBC978-F520-488C-A12B-5597BF499BA1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D0DC12C0-51BE-4482-8D5E-D278D82A451C}"/>
   </bookViews>
@@ -921,7 +921,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0426D88-2664-419A-8274-BC1B5AF433EE}" name="ShortAlarm" displayName="ShortAlarm" ref="A1:C193" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C193" xr:uid="{B0426D88-2664-419A-8274-BC1B5AF433EE}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{26BD7867-3E40-463E-B6ED-4560A82D6BBF}" name="Alarm Text" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{7EBA5675-133D-4AEC-90B7-F43092420BF5}" name="Renamed Alarm" dataDxfId="1"/>
@@ -1251,7 +1250,7 @@
   <dimension ref="A1:C193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A172" sqref="A172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>